<commit_message>
Update build steps for animation
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT-Assessment-Hour-Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7485"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Subject</t>
   </si>
@@ -83,12 +83,6 @@
     <t>After reading the wiki for a little bit, I thought of just going with a naive approach on the algorithm as I've done something similar before, and I didn't see any problems not doing that</t>
   </si>
   <si>
-    <t>Think about general structure</t>
-  </si>
-  <si>
-    <t>I'll probably spend some time here, because I don't have enough experience in Unity and I'll use my previous knowledge on building engines so far to create a quick framework for the visual representation, unfortunately can't use a gpu accelerator yet</t>
-  </si>
-  <si>
     <t>Implementing the framework</t>
   </si>
   <si>
@@ -131,7 +125,28 @@
     <t>Clamp maze dimensions between min and max cells</t>
   </si>
   <si>
-    <t>Framework: porting old code, fixing bugs</t>
+    <t>I'll probably spend some time here, because I don't have enough experience in Unity and I'll use my previous knowledge on building engines so far to create a quick framework for the visual representation, unfortunately can't use a gpu accelerator yet, so it's software rendered</t>
+  </si>
+  <si>
+    <t>14/03/2024</t>
+  </si>
+  <si>
+    <t>14/03/2025</t>
+  </si>
+  <si>
+    <t>14/03/2026</t>
+  </si>
+  <si>
+    <t>14/03/2027</t>
+  </si>
+  <si>
+    <t>14/03/2028</t>
+  </si>
+  <si>
+    <t>Framework: porting old code, adding new features, fixing bugs (total time)</t>
+  </si>
+  <si>
+    <t>Thinking about general structure</t>
   </si>
 </sst>
 </file>
@@ -438,7 +453,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -481,6 +496,9 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -493,8 +511,8 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1755,13 +1773,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.69921875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="41.69921875" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.69921875" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.59765625" style="1" customWidth="1"/>
     <col min="4" max="4" width="108" style="1" customWidth="1"/>
@@ -1770,22 +1788,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1">
-      <c r="A1" s="22"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="10"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="16" t="s">
@@ -1823,114 +1841,126 @@
     </row>
     <row r="5" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="17">
         <v>4</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B6" s="17">
         <v>7</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B7" s="17">
         <v>0.5</v>
       </c>
-      <c r="C7" s="18"/>
+      <c r="C7" s="18" t="s">
+        <v>10</v>
+      </c>
       <c r="D7" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="17">
         <v>0.5</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="D8" s="15"/>
       <c r="E8" s="19"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="17">
         <v>0.5</v>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="D9" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="17">
         <v>0.5</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="D10" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
       </c>
-      <c r="C11" s="18"/>
+      <c r="C11" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="D11" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="26">
+        <v>21</v>
+      </c>
+      <c r="B12" s="22">
         <v>0.5</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="17" t="s">
-        <v>24</v>
+      <c r="C12" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>22</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="4"/>

</xml_diff>